<commit_message>
Dashboard implemented. more features to be added
</commit_message>
<xml_diff>
--- a/Social_Reports/tfvm_report_february_2025_2026-01.xlsx
+++ b/Social_Reports/tfvm_report_february_2025_2026-01.xlsx
@@ -958,7 +958,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N98"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3137,2173 +3137,91 @@
       </c>
       <c r="N45" s="7" t="inlineStr"/>
     </row>
-    <row r="46">
-      <c r="A46" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B46" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="C46" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="D46" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E46" s="7" t="inlineStr">
-        <is>
-          <t>Weekend Shopping Spree</t>
-        </is>
-      </c>
-      <c r="F46" s="4" t="inlineStr">
-        <is>
-          <t>03/02</t>
-        </is>
-      </c>
-      <c r="G46" s="8" t="n">
-        <v>41607</v>
-      </c>
-      <c r="H46" s="9" t="inlineStr"/>
-      <c r="I46" s="9" t="n">
-        <v>3775</v>
-      </c>
-      <c r="J46" s="9" t="n">
-        <v>320</v>
-      </c>
-      <c r="K46" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="L46" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M46" s="9" t="n">
-        <v>36</v>
-      </c>
-      <c r="N46" s="7" t="inlineStr"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B47" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="C47" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="D47" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E47" s="7" t="inlineStr">
-        <is>
-          <t>KOL TikTok – Nina Tomyam Seafood Recipe</t>
-        </is>
-      </c>
-      <c r="F47" s="4" t="inlineStr">
-        <is>
-          <t>07/02</t>
-        </is>
-      </c>
-      <c r="G47" s="9" t="inlineStr"/>
-      <c r="H47" s="8" t="n">
-        <v>58652</v>
-      </c>
-      <c r="I47" s="9" t="inlineStr"/>
-      <c r="J47" s="9" t="n">
-        <v>171</v>
-      </c>
-      <c r="K47" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="L47" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="M47" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="N47" s="7" t="inlineStr"/>
-    </row>
+    <row r="46"/>
+    <row r="47"/>
     <row r="48">
-      <c r="A48" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B48" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="C48" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="D48" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E48" s="7" t="inlineStr">
-        <is>
-          <t>Loyalty Program (Gorme Omura Knife Series)</t>
-        </is>
-      </c>
-      <c r="F48" s="4" t="inlineStr">
-        <is>
-          <t>11/02</t>
-        </is>
-      </c>
-      <c r="G48" s="8" t="n">
-        <v>40415</v>
-      </c>
-      <c r="H48" s="9" t="inlineStr"/>
-      <c r="I48" s="9" t="n">
-        <v>3305</v>
-      </c>
-      <c r="J48" s="9" t="n">
-        <v>551</v>
-      </c>
-      <c r="K48" s="9" t="n">
-        <v>8</v>
-      </c>
-      <c r="L48" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="M48" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="N48" s="7" t="inlineStr"/>
+      <c r="A48" s="12" t="inlineStr">
+        <is>
+          <t>📊 SUMMARY STATISTICS</t>
+        </is>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B49" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="C49" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="D49" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E49" s="7" t="inlineStr">
-        <is>
-          <t>Daily Essentials Grab</t>
-        </is>
-      </c>
-      <c r="F49" s="4" t="inlineStr">
-        <is>
-          <t>17/02</t>
-        </is>
-      </c>
-      <c r="G49" s="8" t="n">
-        <v>44105</v>
-      </c>
-      <c r="H49" s="9" t="inlineStr"/>
-      <c r="I49" s="9" t="n">
-        <v>3418</v>
-      </c>
-      <c r="J49" s="9" t="n">
-        <v>241</v>
-      </c>
-      <c r="K49" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="L49" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M49" s="9" t="n">
-        <v>11</v>
-      </c>
-      <c r="N49" s="7" t="inlineStr"/>
+      <c r="A49" s="13" t="inlineStr">
+        <is>
+          <t>Total Posts</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>44</v>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B50" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="C50" s="5" t="n">
-        <v>49</v>
-      </c>
-      <c r="D50" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E50" s="7" t="inlineStr">
-        <is>
-          <t>KOL TikTok – Nina Cucur Udang Rangup</t>
-        </is>
-      </c>
-      <c r="F50" s="4" t="inlineStr">
-        <is>
-          <t>24/02</t>
-        </is>
-      </c>
-      <c r="G50" s="9" t="inlineStr"/>
-      <c r="H50" s="8" t="n">
-        <v>55705</v>
-      </c>
-      <c r="I50" s="9" t="inlineStr"/>
-      <c r="J50" s="9" t="n">
-        <v>142</v>
-      </c>
-      <c r="K50" s="9" t="n">
-        <v>18</v>
-      </c>
-      <c r="L50" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="M50" s="9" t="n">
-        <v>16</v>
-      </c>
-      <c r="N50" s="7" t="inlineStr"/>
+      <c r="A50" s="13" t="inlineStr">
+        <is>
+          <t>Video Posts</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B51" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="C51" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="D51" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E51" s="7" t="inlineStr">
-        <is>
-          <t>Loyalty Program (Gorme Omura Knife Series)</t>
-        </is>
-      </c>
-      <c r="F51" s="4" t="inlineStr">
-        <is>
-          <t>25/02</t>
-        </is>
-      </c>
-      <c r="G51" s="8" t="n">
-        <v>42212</v>
-      </c>
-      <c r="H51" s="9" t="inlineStr"/>
-      <c r="I51" s="9" t="n">
-        <v>3391</v>
-      </c>
-      <c r="J51" s="9" t="n">
-        <v>337</v>
-      </c>
-      <c r="K51" s="9" t="n">
-        <v>13</v>
-      </c>
-      <c r="L51" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="M51" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="N51" s="7" t="inlineStr"/>
+      <c r="A51" s="13" t="inlineStr">
+        <is>
+          <t>Average Reach</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>50,015</t>
+        </is>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B52" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="C52" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="D52" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E52" s="7" t="inlineStr">
-        <is>
-          <t>Promo Video: Cahaya Ramadan</t>
-        </is>
-      </c>
-      <c r="F52" s="4" t="inlineStr">
-        <is>
-          <t>26/02</t>
-        </is>
-      </c>
-      <c r="G52" s="9" t="inlineStr"/>
-      <c r="H52" s="8" t="n">
-        <v>51012</v>
-      </c>
-      <c r="I52" s="9" t="inlineStr"/>
-      <c r="J52" s="9" t="n">
-        <v>74</v>
-      </c>
-      <c r="K52" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="L52" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M52" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="N52" s="7" t="inlineStr"/>
+      <c r="A52" s="13" t="inlineStr">
+        <is>
+          <t>Average Engagement</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>5,072</t>
+        </is>
+      </c>
     </row>
     <row r="53">
-      <c r="A53" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B53" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="C53" s="5" t="n">
-        <v>52</v>
-      </c>
-      <c r="D53" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E53" s="7" t="inlineStr">
-        <is>
-          <t>Weekend Shopping Spree</t>
-        </is>
-      </c>
-      <c r="F53" s="4" t="inlineStr">
-        <is>
-          <t>03/02</t>
-        </is>
-      </c>
-      <c r="G53" s="8" t="n">
-        <v>11692</v>
-      </c>
-      <c r="H53" s="9" t="inlineStr"/>
-      <c r="I53" s="9" t="n">
-        <v>1008</v>
-      </c>
-      <c r="J53" s="9" t="n">
-        <v>1000</v>
-      </c>
-      <c r="K53" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="L53" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M53" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="N53" s="7" t="inlineStr"/>
+      <c r="A53" s="13" t="inlineStr">
+        <is>
+          <t>Total Engagement</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>96,369</t>
+        </is>
+      </c>
     </row>
     <row r="54">
-      <c r="A54" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B54" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="C54" s="5" t="n">
-        <v>53</v>
-      </c>
-      <c r="D54" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E54" s="7" t="inlineStr">
-        <is>
-          <t>Loyalty Program (Gorme Omura Knife Series)</t>
-        </is>
-      </c>
-      <c r="F54" s="4" t="inlineStr">
-        <is>
-          <t>11/02</t>
-        </is>
-      </c>
-      <c r="G54" s="8" t="n">
-        <v>12157</v>
-      </c>
-      <c r="H54" s="9" t="inlineStr"/>
-      <c r="I54" s="9" t="n">
-        <v>1002</v>
-      </c>
-      <c r="J54" s="9" t="n">
-        <v>952</v>
-      </c>
-      <c r="K54" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L54" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M54" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="N54" s="7" t="inlineStr"/>
-    </row>
-    <row r="55">
-      <c r="A55" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B55" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="C55" s="5" t="n">
-        <v>54</v>
-      </c>
-      <c r="D55" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E55" s="7" t="inlineStr">
-        <is>
-          <t>Daily Essential Grab</t>
-        </is>
-      </c>
-      <c r="F55" s="4" t="inlineStr">
-        <is>
-          <t>17/02</t>
-        </is>
-      </c>
-      <c r="G55" s="8" t="n">
-        <v>12450</v>
-      </c>
-      <c r="H55" s="9" t="inlineStr"/>
-      <c r="I55" s="9" t="n">
-        <v>1025</v>
-      </c>
-      <c r="J55" s="9" t="n">
-        <v>1021</v>
-      </c>
-      <c r="K55" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L55" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M55" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="N55" s="7" t="inlineStr"/>
-    </row>
-    <row r="56">
-      <c r="A56" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B56" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="C56" s="5" t="n">
-        <v>55</v>
-      </c>
-      <c r="D56" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E56" s="7" t="inlineStr">
-        <is>
-          <t>Loyalty Program (Gorme Omura Knife Series)</t>
-        </is>
-      </c>
-      <c r="F56" s="4" t="inlineStr">
-        <is>
-          <t>25/02</t>
-        </is>
-      </c>
-      <c r="G56" s="8" t="n">
-        <v>12913</v>
-      </c>
-      <c r="H56" s="9" t="inlineStr"/>
-      <c r="I56" s="9" t="n">
-        <v>1023</v>
-      </c>
-      <c r="J56" s="9" t="n">
-        <v>1017</v>
-      </c>
-      <c r="K56" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L56" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M56" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="N56" s="7" t="inlineStr"/>
-    </row>
-    <row r="57">
-      <c r="A57" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B57" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="C57" s="5" t="n">
-        <v>56</v>
-      </c>
-      <c r="D57" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E57" s="7" t="inlineStr">
-        <is>
-          <t>Promo Cahaya Ramadan</t>
-        </is>
-      </c>
-      <c r="F57" s="4" t="inlineStr">
-        <is>
-          <t>26/02</t>
-        </is>
-      </c>
-      <c r="G57" s="9" t="inlineStr"/>
-      <c r="H57" s="8" t="n">
-        <v>35810</v>
-      </c>
-      <c r="I57" s="9" t="inlineStr"/>
-      <c r="J57" s="9" t="n">
-        <v>18</v>
-      </c>
-      <c r="K57" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L57" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M57" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N57" s="7" t="inlineStr"/>
-    </row>
-    <row r="58">
-      <c r="A58" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B58" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="C58" s="5" t="n">
-        <v>57</v>
-      </c>
-      <c r="D58" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E58" s="7" t="inlineStr">
-        <is>
-          <t>KOL TikTok – Quesha Back To School Promo</t>
-        </is>
-      </c>
-      <c r="F58" s="4" t="inlineStr">
-        <is>
-          <t>03/02</t>
-        </is>
-      </c>
-      <c r="G58" s="9" t="inlineStr"/>
-      <c r="H58" s="8" t="n">
-        <v>17343</v>
-      </c>
-      <c r="I58" s="9" t="inlineStr"/>
-      <c r="J58" s="9" t="n">
-        <v>180</v>
-      </c>
-      <c r="K58" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="L58" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="M58" s="9" t="n">
-        <v>24</v>
-      </c>
-      <c r="N58" s="7" t="inlineStr"/>
-    </row>
-    <row r="59">
-      <c r="A59" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B59" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="C59" s="5" t="n">
-        <v>58</v>
-      </c>
-      <c r="D59" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E59" s="7" t="inlineStr">
-        <is>
-          <t>KOL TikTok – Nina Tomyam Seafood Recipe</t>
-        </is>
-      </c>
-      <c r="F59" s="4" t="inlineStr">
-        <is>
-          <t>07/02</t>
-        </is>
-      </c>
-      <c r="G59" s="9" t="inlineStr"/>
-      <c r="H59" s="8" t="n">
-        <v>19125</v>
-      </c>
-      <c r="I59" s="9" t="inlineStr"/>
-      <c r="J59" s="9" t="n">
-        <v>461</v>
-      </c>
-      <c r="K59" s="9" t="n">
-        <v>10</v>
-      </c>
-      <c r="L59" s="9" t="n">
-        <v>11</v>
-      </c>
-      <c r="M59" s="9" t="n">
-        <v>50</v>
-      </c>
-      <c r="N59" s="7" t="inlineStr"/>
-    </row>
-    <row r="60">
-      <c r="A60" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B60" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="C60" s="5" t="n">
-        <v>59</v>
-      </c>
-      <c r="D60" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E60" s="7" t="inlineStr">
-        <is>
-          <t>KOL TikTok – Saida Back To School / Promosi Ahli</t>
-        </is>
-      </c>
-      <c r="F60" s="4" t="inlineStr">
-        <is>
-          <t>10/02</t>
-        </is>
-      </c>
-      <c r="G60" s="9" t="inlineStr"/>
-      <c r="H60" s="8" t="n">
-        <v>22053</v>
-      </c>
-      <c r="I60" s="9" t="inlineStr"/>
-      <c r="J60" s="9" t="n">
-        <v>42</v>
-      </c>
-      <c r="K60" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L60" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M60" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="N60" s="7" t="inlineStr"/>
-    </row>
-    <row r="61">
-      <c r="A61" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B61" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="C61" s="5" t="n">
-        <v>60</v>
-      </c>
-      <c r="D61" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E61" s="7" t="inlineStr">
-        <is>
-          <t>KOL TikTok – Anne Weekend Groceries Shopping</t>
-        </is>
-      </c>
-      <c r="F61" s="4" t="inlineStr">
-        <is>
-          <t>10/02</t>
-        </is>
-      </c>
-      <c r="G61" s="9" t="inlineStr"/>
-      <c r="H61" s="8" t="n">
-        <v>28764</v>
-      </c>
-      <c r="I61" s="9" t="inlineStr"/>
-      <c r="J61" s="9" t="n">
-        <v>115</v>
-      </c>
-      <c r="K61" s="9" t="n">
-        <v>8</v>
-      </c>
-      <c r="L61" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="M61" s="9" t="n">
-        <v>12</v>
-      </c>
-      <c r="N61" s="7" t="inlineStr"/>
-    </row>
-    <row r="62">
-      <c r="A62" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B62" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="C62" s="5" t="n">
-        <v>61</v>
-      </c>
-      <c r="D62" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E62" s="7" t="inlineStr">
-        <is>
-          <t>TikTok ASMR – Restock Pantry</t>
-        </is>
-      </c>
-      <c r="F62" s="4" t="inlineStr">
-        <is>
-          <t>14/02</t>
-        </is>
-      </c>
-      <c r="G62" s="9" t="inlineStr"/>
-      <c r="H62" s="8" t="n">
-        <v>23571</v>
-      </c>
-      <c r="I62" s="9" t="inlineStr"/>
-      <c r="J62" s="9" t="n">
-        <v>60</v>
-      </c>
-      <c r="K62" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L62" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="M62" s="9" t="n">
-        <v>9</v>
-      </c>
-      <c r="N62" s="7" t="inlineStr"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B63" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="C63" s="5" t="n">
-        <v>62</v>
-      </c>
-      <c r="D63" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E63" s="7" t="inlineStr">
-        <is>
-          <t>KOL TikTok – Wana Grocery Shopping with 2 Kids</t>
-        </is>
-      </c>
-      <c r="F63" s="4" t="inlineStr">
-        <is>
-          <t>17/02</t>
-        </is>
-      </c>
-      <c r="G63" s="9" t="inlineStr"/>
-      <c r="H63" s="8" t="n">
-        <v>23214</v>
-      </c>
-      <c r="I63" s="9" t="inlineStr"/>
-      <c r="J63" s="9" t="n">
-        <v>69</v>
-      </c>
-      <c r="K63" s="9" t="n">
-        <v>16</v>
-      </c>
-      <c r="L63" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M63" s="9" t="n">
-        <v>14</v>
-      </c>
-      <c r="N63" s="7" t="inlineStr"/>
-    </row>
-    <row r="64">
-      <c r="A64" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B64" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="C64" s="5" t="n">
-        <v>63</v>
-      </c>
-      <c r="D64" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E64" s="7" t="inlineStr">
-        <is>
-          <t>TikTok Video – Dua Lipa Trend</t>
-        </is>
-      </c>
-      <c r="F64" s="4" t="inlineStr">
-        <is>
-          <t>24/02</t>
-        </is>
-      </c>
-      <c r="G64" s="9" t="inlineStr"/>
-      <c r="H64" s="8" t="n">
-        <v>45424</v>
-      </c>
-      <c r="I64" s="9" t="inlineStr"/>
-      <c r="J64" s="9" t="n">
-        <v>89</v>
-      </c>
-      <c r="K64" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L64" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M64" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="N64" s="7" t="inlineStr"/>
-    </row>
-    <row r="65">
-      <c r="A65" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B65" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="C65" s="5" t="n">
-        <v>64</v>
-      </c>
-      <c r="D65" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E65" s="7" t="inlineStr">
-        <is>
-          <t>KOL TikTok – Nina Cucur Udang Rangup</t>
-        </is>
-      </c>
-      <c r="F65" s="4" t="inlineStr">
-        <is>
-          <t>24/02</t>
-        </is>
-      </c>
-      <c r="G65" s="9" t="inlineStr"/>
-      <c r="H65" s="8" t="n">
-        <v>12631</v>
-      </c>
-      <c r="I65" s="9" t="inlineStr"/>
-      <c r="J65" s="9" t="n">
-        <v>382</v>
-      </c>
-      <c r="K65" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="L65" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="M65" s="9" t="n">
-        <v>50</v>
-      </c>
-      <c r="N65" s="7" t="inlineStr"/>
-    </row>
-    <row r="66">
-      <c r="A66" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B66" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="C66" s="5" t="n">
-        <v>65</v>
-      </c>
-      <c r="D66" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E66" s="7" t="inlineStr">
-        <is>
-          <t>TikTok Video – TFVM ada Produk Sendiri</t>
-        </is>
-      </c>
-      <c r="F66" s="4" t="inlineStr">
-        <is>
-          <t>26/02</t>
-        </is>
-      </c>
-      <c r="G66" s="9" t="inlineStr"/>
-      <c r="H66" s="8" t="n">
-        <v>22018</v>
-      </c>
-      <c r="I66" s="9" t="inlineStr"/>
-      <c r="J66" s="9" t="n">
-        <v>38</v>
-      </c>
-      <c r="K66" s="9" t="n">
-        <v>10</v>
-      </c>
-      <c r="L66" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="M66" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="N66" s="7" t="inlineStr"/>
-    </row>
-    <row r="67">
-      <c r="A67" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B67" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="C67" s="5" t="n">
-        <v>66</v>
-      </c>
-      <c r="D67" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E67" s="7" t="inlineStr">
-        <is>
-          <t>Weekend Shopping Spree</t>
-        </is>
-      </c>
-      <c r="F67" s="4" t="inlineStr">
-        <is>
-          <t>03/02</t>
-        </is>
-      </c>
-      <c r="G67" s="8" t="n">
-        <v>49275</v>
-      </c>
-      <c r="H67" s="9" t="inlineStr"/>
-      <c r="I67" s="9" t="n">
-        <v>4306</v>
-      </c>
-      <c r="J67" s="9" t="n">
-        <v>237</v>
-      </c>
-      <c r="K67" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L67" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M67" s="9" t="n">
-        <v>21</v>
-      </c>
-      <c r="N67" s="7" t="inlineStr"/>
-    </row>
-    <row r="68">
-      <c r="A68" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B68" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="C68" s="5" t="n">
-        <v>67</v>
-      </c>
-      <c r="D68" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E68" s="7" t="inlineStr">
-        <is>
-          <t>Weekend Shopping Spree</t>
-        </is>
-      </c>
-      <c r="F68" s="4" t="inlineStr">
-        <is>
-          <t>03/02</t>
-        </is>
-      </c>
-      <c r="G68" s="8" t="n">
-        <v>41113</v>
-      </c>
-      <c r="H68" s="9" t="inlineStr"/>
-      <c r="I68" s="9" t="n">
-        <v>3558</v>
-      </c>
-      <c r="J68" s="9" t="n">
-        <v>206</v>
-      </c>
-      <c r="K68" s="9" t="n">
-        <v>9</v>
-      </c>
-      <c r="L68" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M68" s="9" t="n">
-        <v>20</v>
-      </c>
-      <c r="N68" s="7" t="inlineStr"/>
-    </row>
-    <row r="69">
-      <c r="A69" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B69" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="C69" s="5" t="n">
-        <v>68</v>
-      </c>
-      <c r="D69" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E69" s="7" t="inlineStr">
-        <is>
-          <t>Nina Tomyam Seafood Recipe</t>
-        </is>
-      </c>
-      <c r="F69" s="4" t="inlineStr">
-        <is>
-          <t>07/02</t>
-        </is>
-      </c>
-      <c r="G69" s="8" t="n">
-        <v>47133</v>
-      </c>
-      <c r="H69" s="9" t="inlineStr"/>
-      <c r="I69" s="9" t="n">
-        <v>4132</v>
-      </c>
-      <c r="J69" s="9" t="n">
-        <v>496</v>
-      </c>
-      <c r="K69" s="9" t="n">
-        <v>11</v>
-      </c>
-      <c r="L69" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M69" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N69" s="7" t="inlineStr"/>
-    </row>
-    <row r="70">
-      <c r="A70" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B70" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="C70" s="5" t="n">
-        <v>69</v>
-      </c>
-      <c r="D70" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E70" s="7" t="inlineStr">
-        <is>
-          <t>Loyalty Program – Gorme Omura Knife Series</t>
-        </is>
-      </c>
-      <c r="F70" s="4" t="inlineStr">
-        <is>
-          <t>11/02</t>
-        </is>
-      </c>
-      <c r="G70" s="8" t="n">
-        <v>44547</v>
-      </c>
-      <c r="H70" s="9" t="inlineStr"/>
-      <c r="I70" s="9" t="n">
-        <v>3408</v>
-      </c>
-      <c r="J70" s="9" t="n">
-        <v>470</v>
-      </c>
-      <c r="K70" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="L70" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="M70" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="N70" s="7" t="inlineStr"/>
-    </row>
-    <row r="71">
-      <c r="A71" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B71" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="C71" s="5" t="n">
-        <v>70</v>
-      </c>
-      <c r="D71" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E71" s="7" t="inlineStr">
-        <is>
-          <t>Loyalty Program – Gorme Omura Knife Series</t>
-        </is>
-      </c>
-      <c r="F71" s="4" t="inlineStr">
-        <is>
-          <t>11/02</t>
-        </is>
-      </c>
-      <c r="G71" s="9" t="inlineStr"/>
-      <c r="H71" s="8" t="n">
-        <v>131496</v>
-      </c>
-      <c r="I71" s="9" t="inlineStr"/>
-      <c r="J71" s="9" t="n">
-        <v>481</v>
-      </c>
-      <c r="K71" s="9" t="n">
-        <v>21</v>
-      </c>
-      <c r="L71" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="M71" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N71" s="7" t="inlineStr"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B72" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="C72" s="5" t="n">
-        <v>71</v>
-      </c>
-      <c r="D72" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E72" s="7" t="inlineStr">
-        <is>
-          <t>TikTok ASMR – Restock Pantry</t>
-        </is>
-      </c>
-      <c r="F72" s="4" t="inlineStr">
-        <is>
-          <t>14/02</t>
-        </is>
-      </c>
-      <c r="G72" s="9" t="inlineStr"/>
-      <c r="H72" s="8" t="n">
-        <v>51093</v>
-      </c>
-      <c r="I72" s="9" t="inlineStr"/>
-      <c r="J72" s="9" t="n">
-        <v>81</v>
-      </c>
-      <c r="K72" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L72" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M72" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N72" s="7" t="inlineStr"/>
-    </row>
-    <row r="73">
-      <c r="A73" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B73" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="C73" s="5" t="n">
-        <v>72</v>
-      </c>
-      <c r="D73" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E73" s="7" t="inlineStr">
-        <is>
-          <t>Daily Essential Grab</t>
-        </is>
-      </c>
-      <c r="F73" s="4" t="inlineStr">
-        <is>
-          <t>22/02</t>
-        </is>
-      </c>
-      <c r="G73" s="8" t="n">
-        <v>40740</v>
-      </c>
-      <c r="H73" s="9" t="inlineStr"/>
-      <c r="I73" s="9" t="n">
-        <v>3350</v>
-      </c>
-      <c r="J73" s="9" t="n">
-        <v>88</v>
-      </c>
-      <c r="K73" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L73" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M73" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N73" s="7" t="inlineStr"/>
-    </row>
-    <row r="74">
-      <c r="A74" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B74" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="C74" s="5" t="n">
-        <v>73</v>
-      </c>
-      <c r="D74" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E74" s="7" t="inlineStr">
-        <is>
-          <t>Daily Essential Grab</t>
-        </is>
-      </c>
-      <c r="F74" s="4" t="inlineStr">
-        <is>
-          <t>22/02</t>
-        </is>
-      </c>
-      <c r="G74" s="8" t="n">
-        <v>42339</v>
-      </c>
-      <c r="H74" s="9" t="inlineStr"/>
-      <c r="I74" s="9" t="n">
-        <v>3425</v>
-      </c>
-      <c r="J74" s="9" t="n">
-        <v>184</v>
-      </c>
-      <c r="K74" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L74" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M74" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N74" s="7" t="inlineStr"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B75" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="C75" s="5" t="n">
-        <v>74</v>
-      </c>
-      <c r="D75" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E75" s="7" t="inlineStr">
-        <is>
-          <t>Nina – Cucur Udang Rangup</t>
-        </is>
-      </c>
-      <c r="F75" s="4" t="inlineStr">
-        <is>
-          <t>24/02</t>
-        </is>
-      </c>
-      <c r="G75" s="9" t="inlineStr"/>
-      <c r="H75" s="8" t="n">
-        <v>50440</v>
-      </c>
-      <c r="I75" s="9" t="inlineStr"/>
-      <c r="J75" s="9" t="n">
-        <v>33</v>
-      </c>
-      <c r="K75" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="L75" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M75" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="N75" s="7" t="inlineStr"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B76" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="C76" s="5" t="n">
-        <v>75</v>
-      </c>
-      <c r="D76" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E76" s="7" t="inlineStr">
-        <is>
-          <t>TikTok Video – Dua Lipa Trend</t>
-        </is>
-      </c>
-      <c r="F76" s="4" t="inlineStr">
-        <is>
-          <t>24/02</t>
-        </is>
-      </c>
-      <c r="G76" s="9" t="inlineStr"/>
-      <c r="H76" s="8" t="n">
-        <v>50719</v>
-      </c>
-      <c r="I76" s="9" t="inlineStr"/>
-      <c r="J76" s="9" t="n">
-        <v>8</v>
-      </c>
-      <c r="K76" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L76" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M76" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N76" s="7" t="inlineStr"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B77" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="C77" s="5" t="n">
-        <v>76</v>
-      </c>
-      <c r="D77" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E77" s="7" t="inlineStr">
-        <is>
-          <t>Loyalty Program – Gorme Omura Knife Series</t>
-        </is>
-      </c>
-      <c r="F77" s="4" t="inlineStr">
-        <is>
-          <t>25/02</t>
-        </is>
-      </c>
-      <c r="G77" s="8" t="n">
-        <v>41788</v>
-      </c>
-      <c r="H77" s="9" t="inlineStr"/>
-      <c r="I77" s="9" t="n">
-        <v>4215</v>
-      </c>
-      <c r="J77" s="9" t="n">
-        <v>268</v>
-      </c>
-      <c r="K77" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L77" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="M77" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N77" s="7" t="inlineStr"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B78" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="C78" s="5" t="n">
-        <v>77</v>
-      </c>
-      <c r="D78" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E78" s="7" t="inlineStr">
-        <is>
-          <t>Loyalty Program – Gorme Omura Knife Series</t>
-        </is>
-      </c>
-      <c r="F78" s="4" t="inlineStr">
-        <is>
-          <t>25/02</t>
-        </is>
-      </c>
-      <c r="G78" s="8" t="n">
-        <v>42824</v>
-      </c>
-      <c r="H78" s="9" t="inlineStr"/>
-      <c r="I78" s="9" t="n">
-        <v>3395</v>
-      </c>
-      <c r="J78" s="9" t="n">
-        <v>353</v>
-      </c>
-      <c r="K78" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="L78" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="M78" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N78" s="7" t="inlineStr"/>
-    </row>
-    <row r="79">
-      <c r="A79" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B79" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="C79" s="5" t="n">
-        <v>78</v>
-      </c>
-      <c r="D79" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E79" s="7" t="inlineStr">
-        <is>
-          <t>TikTok Video – TFVM ada Produk Sendiri</t>
-        </is>
-      </c>
-      <c r="F79" s="4" t="inlineStr">
-        <is>
-          <t>26/02</t>
-        </is>
-      </c>
-      <c r="G79" s="9" t="inlineStr"/>
-      <c r="H79" s="8" t="n">
-        <v>50582</v>
-      </c>
-      <c r="I79" s="9" t="inlineStr"/>
-      <c r="J79" s="9" t="n">
-        <v>34</v>
-      </c>
-      <c r="K79" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L79" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M79" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N79" s="7" t="inlineStr"/>
-    </row>
-    <row r="80">
-      <c r="A80" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B80" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="C80" s="5" t="n">
-        <v>79</v>
-      </c>
-      <c r="D80" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E80" s="7" t="inlineStr">
-        <is>
-          <t>Promo Video: Cahaya Ramadan</t>
-        </is>
-      </c>
-      <c r="F80" s="4" t="inlineStr">
-        <is>
-          <t>26/02</t>
-        </is>
-      </c>
-      <c r="G80" s="9" t="inlineStr"/>
-      <c r="H80" s="8" t="n">
-        <v>51285</v>
-      </c>
-      <c r="I80" s="9" t="inlineStr"/>
-      <c r="J80" s="9" t="n">
-        <v>23</v>
-      </c>
-      <c r="K80" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L80" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M80" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="N80" s="7" t="inlineStr"/>
-    </row>
-    <row r="81">
-      <c r="A81" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B81" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="C81" s="5" t="n">
-        <v>80</v>
-      </c>
-      <c r="D81" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E81" s="7" t="inlineStr">
-        <is>
-          <t>Promo Video: Cahaya Ramadan</t>
-        </is>
-      </c>
-      <c r="F81" s="4" t="inlineStr">
-        <is>
-          <t>26/02</t>
-        </is>
-      </c>
-      <c r="G81" s="9" t="inlineStr"/>
-      <c r="H81" s="8" t="n">
-        <v>50209</v>
-      </c>
-      <c r="I81" s="9" t="inlineStr"/>
-      <c r="J81" s="9" t="n">
-        <v>30</v>
-      </c>
-      <c r="K81" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L81" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M81" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N81" s="7" t="inlineStr"/>
-    </row>
-    <row r="82">
-      <c r="A82" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B82" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="C82" s="5" t="n">
-        <v>81</v>
-      </c>
-      <c r="D82" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E82" s="7" t="inlineStr">
-        <is>
-          <t>Quesha: Back to School</t>
-        </is>
-      </c>
-      <c r="F82" s="4" t="inlineStr">
-        <is>
-          <t>03/02</t>
-        </is>
-      </c>
-      <c r="G82" s="9" t="inlineStr"/>
-      <c r="H82" s="8" t="n">
-        <v>10307</v>
-      </c>
-      <c r="I82" s="9" t="inlineStr"/>
-      <c r="J82" s="9" t="n">
-        <v>225</v>
-      </c>
-      <c r="K82" s="9" t="n">
-        <v>9</v>
-      </c>
-      <c r="L82" s="9" t="n">
-        <v>41</v>
-      </c>
-      <c r="M82" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="N82" s="11" t="inlineStr">
-        <is>
-          <t>https://www.instagram.com/p/DFmlwmaTHdI</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B83" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="C83" s="5" t="n">
-        <v>82</v>
-      </c>
-      <c r="D83" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E83" s="7" t="inlineStr">
-        <is>
-          <t>Nina: Tomyam Seafood Recipe</t>
-        </is>
-      </c>
-      <c r="F83" s="4" t="inlineStr">
-        <is>
-          <t>07/02</t>
-        </is>
-      </c>
-      <c r="G83" s="9" t="inlineStr"/>
-      <c r="H83" s="8" t="n">
-        <v>35536</v>
-      </c>
-      <c r="I83" s="9" t="inlineStr"/>
-      <c r="J83" s="9" t="n">
-        <v>605</v>
-      </c>
-      <c r="K83" s="9" t="n">
-        <v>658</v>
-      </c>
-      <c r="L83" s="9" t="n">
-        <v>16</v>
-      </c>
-      <c r="M83" s="9" t="n">
-        <v>252</v>
-      </c>
-      <c r="N83" s="11" t="inlineStr">
-        <is>
-          <t>https://www.instagram.com/p/DFws0PizSyc</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B84" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="C84" s="5" t="n">
-        <v>83</v>
-      </c>
-      <c r="D84" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E84" s="7" t="inlineStr">
-        <is>
-          <t>Saida: Back to School/ Promosi Ahli</t>
-        </is>
-      </c>
-      <c r="F84" s="4" t="inlineStr">
-        <is>
-          <t>10/02</t>
-        </is>
-      </c>
-      <c r="G84" s="9" t="inlineStr"/>
-      <c r="H84" s="9" t="n">
-        <v>3253</v>
-      </c>
-      <c r="I84" s="9" t="inlineStr"/>
-      <c r="J84" s="9" t="n">
-        <v>326</v>
-      </c>
-      <c r="K84" s="9" t="n">
-        <v>22</v>
-      </c>
-      <c r="L84" s="9" t="n">
-        <v>9</v>
-      </c>
-      <c r="M84" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="N84" s="11" t="inlineStr">
-        <is>
-          <t>https://www.instagram.com/reel/DF4rOJ5pd-b</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B85" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="C85" s="5" t="n">
-        <v>84</v>
-      </c>
-      <c r="D85" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E85" s="7" t="inlineStr">
-        <is>
-          <t>Wana: Grocery Shopping with 2 Kids</t>
-        </is>
-      </c>
-      <c r="F85" s="4" t="inlineStr">
-        <is>
-          <t>15/02</t>
-        </is>
-      </c>
-      <c r="G85" s="9" t="inlineStr"/>
-      <c r="H85" s="9" t="n">
-        <v>2186</v>
-      </c>
-      <c r="I85" s="9" t="inlineStr"/>
-      <c r="J85" s="9" t="n">
-        <v>127</v>
-      </c>
-      <c r="K85" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L85" s="9" t="n">
-        <v>64</v>
-      </c>
-      <c r="M85" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="N85" s="11" t="inlineStr">
-        <is>
-          <t>https://www.instagram.com/reel/DGFt7mBy5Rf</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B86" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="C86" s="5" t="n">
-        <v>85</v>
-      </c>
-      <c r="D86" s="10" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="E86" s="7" t="inlineStr">
-        <is>
-          <t>Nina: Cucur Udang Rangup</t>
-        </is>
-      </c>
-      <c r="F86" s="4" t="inlineStr">
-        <is>
-          <t>24/02</t>
-        </is>
-      </c>
-      <c r="G86" s="9" t="inlineStr"/>
-      <c r="H86" s="8" t="n">
-        <v>42767</v>
-      </c>
-      <c r="I86" s="9" t="inlineStr"/>
-      <c r="J86" s="9" t="n">
-        <v>694</v>
-      </c>
-      <c r="K86" s="9" t="n">
-        <v>299</v>
-      </c>
-      <c r="L86" s="9" t="n">
-        <v>18</v>
-      </c>
-      <c r="M86" s="9" t="n">
-        <v>791</v>
-      </c>
-      <c r="N86" s="11" t="inlineStr">
-        <is>
-          <t>https://www.instagram.com/p/DGdSCbmTSKZ</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B87" s="5" t="n">
-        <v>79</v>
-      </c>
-      <c r="C87" s="5" t="n">
-        <v>86</v>
-      </c>
-      <c r="D87" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E87" s="7" t="inlineStr">
-        <is>
-          <t>Selamat Hari Valentine</t>
-        </is>
-      </c>
-      <c r="F87" s="4" t="inlineStr">
-        <is>
-          <t>05/02</t>
-        </is>
-      </c>
-      <c r="G87" s="8" t="n">
-        <v>93349</v>
-      </c>
-      <c r="H87" s="9" t="inlineStr"/>
-      <c r="I87" s="9" t="n">
-        <v>4147</v>
-      </c>
-      <c r="J87" s="9" t="n">
-        <v>538</v>
-      </c>
-      <c r="K87" s="9" t="n">
-        <v>16</v>
-      </c>
-      <c r="L87" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="M87" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="N87" s="7" t="inlineStr"/>
-    </row>
-    <row r="88">
-      <c r="A88" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B88" s="5" t="n">
-        <v>79</v>
-      </c>
-      <c r="C88" s="5" t="n">
-        <v>87</v>
-      </c>
-      <c r="D88" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E88" s="7" t="inlineStr">
-        <is>
-          <t>Cahaya Ramadan</t>
-        </is>
-      </c>
-      <c r="F88" s="4" t="inlineStr">
-        <is>
-          <t>24/02</t>
-        </is>
-      </c>
-      <c r="G88" s="8" t="n">
-        <v>151263</v>
-      </c>
-      <c r="H88" s="9" t="inlineStr"/>
-      <c r="I88" s="8" t="n">
-        <v>33779</v>
-      </c>
-      <c r="J88" s="9" t="n">
-        <v>965</v>
-      </c>
-      <c r="K88" s="9" t="n">
-        <v>232</v>
-      </c>
-      <c r="L88" s="9" t="n">
-        <v>11</v>
-      </c>
-      <c r="M88" s="9" t="n">
-        <v>29</v>
-      </c>
-      <c r="N88" s="7" t="inlineStr"/>
-    </row>
-    <row r="89">
-      <c r="A89" s="4" t="inlineStr">
-        <is>
-          <t>TFVM_REPORT (MARCH 2025).pptx</t>
-        </is>
-      </c>
-      <c r="B89" s="5" t="n">
-        <v>79</v>
-      </c>
-      <c r="C89" s="5" t="n">
-        <v>88</v>
-      </c>
-      <c r="D89" s="6" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="E89" s="7" t="inlineStr">
-        <is>
-          <t>Tawaran Istimewa 4 Hari</t>
-        </is>
-      </c>
-      <c r="F89" s="4" t="inlineStr">
-        <is>
-          <t>26/02</t>
-        </is>
-      </c>
-      <c r="G89" s="8" t="n">
-        <v>138367</v>
-      </c>
-      <c r="H89" s="9" t="inlineStr"/>
-      <c r="I89" s="8" t="n">
-        <v>10707</v>
-      </c>
-      <c r="J89" s="9" t="n">
-        <v>541</v>
-      </c>
-      <c r="K89" s="9" t="n">
-        <v>28</v>
-      </c>
-      <c r="L89" s="9" t="n">
-        <v>13</v>
-      </c>
-      <c r="M89" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="N89" s="7" t="inlineStr"/>
-    </row>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92">
-      <c r="A92" s="12" t="inlineStr">
-        <is>
-          <t>📊 SUMMARY STATISTICS</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="13" t="inlineStr">
-        <is>
-          <t>Total Posts</t>
-        </is>
-      </c>
-      <c r="B93" t="n">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="13" t="inlineStr">
-        <is>
-          <t>Video Posts</t>
-        </is>
-      </c>
-      <c r="B94" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="13" t="inlineStr">
-        <is>
-          <t>Average Reach</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>50,015</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="13" t="inlineStr">
-        <is>
-          <t>Average Engagement</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>5,072</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="13" t="inlineStr">
-        <is>
-          <t>Total Engagement</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>192,738</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="13" t="inlineStr">
+      <c r="A54" s="13" t="inlineStr">
         <is>
           <t>Post Types</t>
         </is>
       </c>
-      <c r="B98" s="13" t="inlineStr">
-        <is>
-          <t>Video: 50</t>
-        </is>
-      </c>
-      <c r="C98" s="13" t="inlineStr">
-        <is>
-          <t>Post: 38</t>
+      <c r="B54" s="13" t="inlineStr">
+        <is>
+          <t>Video: 25</t>
+        </is>
+      </c>
+      <c r="C54" s="13" t="inlineStr">
+        <is>
+          <t>Post: 19</t>
         </is>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:N1"/>
-  <conditionalFormatting sqref="I2:I89">
+  <conditionalFormatting sqref="I2:I45">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -5318,7 +3236,7 @@
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D89">
+  <conditionalFormatting sqref="D2:D45">
     <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
       <formula>"Video"</formula>
     </cfRule>
@@ -5329,11 +3247,6 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N40" r:id="rId3"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N41" r:id="rId4"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N42" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N82" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N83" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N84" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N85" r:id="rId9"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N86" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5367,7 +3280,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
@@ -5377,7 +3290,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15">
@@ -5400,91 +3313,91 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Cahaya Ramadan</t>
+          <t>Tawaran Istimewa 4 Hari</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>33779</v>
+        <v>10707</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Tawaran Istimewa 4 Hari</t>
+          <t>Weekend Shopping Spree</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>10707</v>
+        <v>4306</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Tawaran Istimewa 4 Hari</t>
+          <t>Loyalty Program – Gorme Omura ...</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>10707</v>
+        <v>4215</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Weekend Shopping Spree</t>
+          <t>Selamat Hari Valentine</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>4306</v>
+        <v>4147</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Weekend Shopping Spree</t>
+          <t>Nina Tomyam Seafood Recipe</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>4306</v>
+        <v>4132</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Loyalty Program – Gorme Omura ...</t>
+          <t>Weekend Shopping Spree</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>4215</v>
+        <v>3775</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Loyalty Program – Gorme Omura ...</t>
+          <t>Weekend Shopping Spree</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>4215</v>
+        <v>3558</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Selamat Hari Valentine</t>
+          <t>Daily Essential Grab</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>4147</v>
+        <v>3425</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Selamat Hari Valentine</t>
+          <t>Daily Essentials Grab</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>4147</v>
+        <v>3418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>